<commit_message>
change eq. rate 20
change eq. model 6,7
rate 20
</commit_message>
<xml_diff>
--- a/pca_table.xlsx
+++ b/pca_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://masseyuni-my.sharepoint.com/personal/whorpien_massey_ac_nz/Documents/InfectiousModel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="105" documentId="8_{474EAB77-0A58-8D4B-B89B-7202EEF086C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFFA5685-FC53-A543-BD9D-B2A4BFDD3C4E}"/>
+  <xr:revisionPtr revIDLastSave="204" documentId="8_{474EAB77-0A58-8D4B-B89B-7202EEF086C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62BEC024-1633-41E6-91B6-4262325D6620}"/>
   <bookViews>
-    <workbookView xWindow="41560" yWindow="-1400" windowWidth="25460" windowHeight="21440" activeTab="1" xr2:uid="{801422A5-DD4D-ED4E-BCEE-D365A9AA47EB}"/>
+    <workbookView xWindow="75" yWindow="0" windowWidth="28440" windowHeight="16050" xr2:uid="{801422A5-DD4D-ED4E-BCEE-D365A9AA47EB}"/>
   </bookViews>
   <sheets>
     <sheet name="norm" sheetId="1" r:id="rId1"/>
@@ -229,7 +229,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -256,6 +256,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -277,12 +293,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,1145 +616,1146 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F095E656-8A54-F542-A328-8135B2ED3A27}">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:H1048576"/>
+    <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="4"/>
-    <col min="4" max="4" width="8.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="4"/>
-    <col min="6" max="6" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="4"/>
+    <col min="1" max="1" width="23.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.875" style="4"/>
+    <col min="5" max="5" width="8.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1">
         <v>3.3300000000000003E-5</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C2" s="1">
         <v>7.1428599999999995E-2</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
         <v>51.186666670000001</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="H2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1">
         <v>4.7999999999999998E-6</v>
       </c>
-      <c r="B3" s="1">
+      <c r="C3" s="1">
         <v>6.6667000000000002E-3</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>2.7399999999999999E-5</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>0.11</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F3" s="3">
         <v>-56.466667000000001</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+      <c r="H3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1">
         <v>1.4333E-3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="C4" s="1">
         <v>6.6667000000000002E-3</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>2.7399999999999999E-5</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>0.11</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>-89.3</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="H4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1">
         <v>2.0999999999999999E-5</v>
       </c>
-      <c r="B5" s="1">
+      <c r="C5" s="1">
         <v>6.6667000000000002E-3</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>2.7399999999999999E-5</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>0.11</v>
       </c>
-      <c r="E5" s="3">
+      <c r="F5" s="3">
         <v>-84.096666999999997</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+      <c r="H5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1">
         <v>2.6999999999999999E-5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="C6" s="1">
         <v>6.6667000000000002E-3</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>2.7399999999999999E-5</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>0.11</v>
       </c>
-      <c r="E6" s="3">
+      <c r="F6" s="3">
         <v>-86.003332999999998</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+      <c r="H6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1">
         <v>0.33500000000000002</v>
       </c>
-      <c r="B7" s="1">
+      <c r="C7" s="1">
         <v>0.3</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>0.33333000000000002</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>5.1999999999999995E-4</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="6">
         <v>47.466666670000002</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+      <c r="G7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1">
         <v>0.33500000000000002</v>
       </c>
-      <c r="B8" s="1">
+      <c r="C8" s="1">
         <v>0.3</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <v>0.33333000000000002</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="6">
         <v>-84.14</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+      <c r="G8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="1">
         <v>0.55000000000000004</v>
       </c>
-      <c r="B9" s="1">
+      <c r="C9" s="1">
         <v>0.3</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D9" s="1">
         <v>0.33333000000000002</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>5.1999999999999995E-4</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="6">
         <v>45.81</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+      <c r="G9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="1">
         <v>0.55000000000000004</v>
       </c>
-      <c r="B10" s="1">
+      <c r="C10" s="1">
         <v>0.3</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
         <v>0.33333000000000002</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="6">
         <v>-85.636666669999997</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
+      <c r="G10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1">
         <v>1.1167E-3</v>
       </c>
-      <c r="B11" s="1">
+      <c r="C11" s="1">
         <v>0.3</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
         <v>0.33333000000000002</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>5.1999999999999995E-4</v>
       </c>
-      <c r="E11" s="3">
+      <c r="F11" s="7">
         <v>148.63666699999999</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
+      <c r="G11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1">
         <v>1.1167E-3</v>
       </c>
-      <c r="B12" s="1">
+      <c r="C12" s="1">
         <v>0.3</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="1">
         <v>0.33333000000000002</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="E12" s="3">
+      <c r="F12" s="7">
         <v>19.7233333</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
+      <c r="G12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="1">
         <v>1.8332999999999999E-3</v>
       </c>
-      <c r="B13" s="1">
+      <c r="C13" s="1">
         <v>0.3</v>
       </c>
-      <c r="C13" s="1">
+      <c r="D13" s="1">
         <v>0.33333000000000002</v>
       </c>
-      <c r="D13" s="1">
+      <c r="E13" s="1">
         <v>5.1999999999999995E-4</v>
       </c>
-      <c r="E13" s="3">
+      <c r="F13" s="7">
         <v>127.07</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
+      <c r="G13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1">
         <v>1.8332999999999999E-3</v>
       </c>
-      <c r="B14" s="1">
+      <c r="C14" s="1">
         <v>0.3</v>
       </c>
-      <c r="C14" s="1">
+      <c r="D14" s="1">
         <v>0.33333000000000002</v>
       </c>
-      <c r="D14" s="1">
+      <c r="E14" s="1">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="E14" s="3">
+      <c r="F14" s="7">
         <v>148.63666699999999</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
+      <c r="G14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="1">
         <v>1.0670000000000001E-4</v>
       </c>
-      <c r="B15" s="1">
+      <c r="C15" s="1">
         <v>0.14285999999999999</v>
       </c>
-      <c r="C15" s="1">
+      <c r="D15" s="1">
         <v>2.8570000000000002E-2</v>
       </c>
-      <c r="D15" s="1">
+      <c r="E15" s="1">
         <v>0.01</v>
       </c>
-      <c r="E15" s="1">
+      <c r="F15" s="1">
         <v>45.193333330000002</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="H15" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="1">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="B16" s="1">
+      <c r="C16" s="1">
         <v>0.14285999999999999</v>
       </c>
-      <c r="C16" s="1">
+      <c r="D16" s="1">
         <v>2.8570000000000002E-2</v>
       </c>
-      <c r="D16" s="1">
+      <c r="E16" s="1">
         <v>0.01</v>
       </c>
-      <c r="E16" s="1">
+      <c r="F16" s="1">
         <v>-85.233333329999994</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="H16" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="1">
         <v>3.8329999999999999E-4</v>
       </c>
-      <c r="B17" s="1">
+      <c r="C17" s="1">
         <v>0.16667000000000001</v>
       </c>
-      <c r="C17" s="1">
+      <c r="D17" s="1">
         <v>0.2</v>
       </c>
-      <c r="D17" s="1">
+      <c r="E17" s="1">
         <v>0.03</v>
       </c>
-      <c r="E17" s="1">
+      <c r="F17" s="1">
         <v>163.44333330000001</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="H17" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="1">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="B18" s="1">
+      <c r="C18" s="1">
         <v>0.16667000000000001</v>
       </c>
-      <c r="C18" s="1">
+      <c r="D18" s="1">
         <v>0.2</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E18" s="1">
         <v>0.03</v>
       </c>
-      <c r="E18" s="1">
+      <c r="F18" s="1">
         <v>-64.48</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="H18" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="1">
         <v>7.2800000000000004E-2</v>
       </c>
-      <c r="B19" s="1">
+      <c r="C19" s="1">
         <v>0.16667000000000001</v>
       </c>
-      <c r="C19" s="1">
+      <c r="D19" s="1">
         <v>0.2</v>
       </c>
-      <c r="D19" s="1">
+      <c r="E19" s="1">
         <v>0.03</v>
       </c>
-      <c r="E19" s="1">
+      <c r="F19" s="1">
         <v>-71.27</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="H19" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="1">
         <v>21.84</v>
       </c>
-      <c r="B20" s="1">
+      <c r="C20" s="1">
         <v>0.16667000000000001</v>
       </c>
-      <c r="C20" s="1">
+      <c r="D20" s="1">
         <v>0.2</v>
       </c>
-      <c r="D20" s="1">
+      <c r="E20" s="1">
         <v>0.03</v>
       </c>
-      <c r="E20" s="1">
+      <c r="F20" s="1">
         <v>-80.236666670000005</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="H20" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="1">
         <v>5.4999999999999999E-6</v>
       </c>
-      <c r="B21" s="1">
+      <c r="C21" s="1">
         <v>7.1429999999999993E-2</v>
       </c>
-      <c r="C21" s="1">
+      <c r="D21" s="1">
         <v>1.3699000000000001E-3</v>
       </c>
-      <c r="D21" s="1">
+      <c r="E21" s="1">
         <v>0.03</v>
       </c>
-      <c r="E21" s="1">
+      <c r="F21" s="1">
         <v>13.72666667</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="H21" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="1">
         <v>1.8300000000000001E-5</v>
       </c>
-      <c r="B22" s="1">
+      <c r="C22" s="1">
         <v>7.1429999999999993E-2</v>
       </c>
-      <c r="C22" s="1">
+      <c r="D22" s="1">
         <v>1.3699000000000001E-3</v>
       </c>
-      <c r="D22" s="1">
+      <c r="E22" s="1">
         <v>0.03</v>
       </c>
-      <c r="E22" s="1">
+      <c r="F22" s="1">
         <v>-66.403333329999995</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="H22" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="1">
         <v>0.01</v>
       </c>
-      <c r="B23" s="1">
+      <c r="C23" s="1">
         <v>7.1428599999999995E-2</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
       </c>
       <c r="E23" s="1">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1">
         <v>56.93</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="H23" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="1">
         <v>1.4333E-3</v>
       </c>
-      <c r="B24" s="1">
+      <c r="C24" s="1">
         <v>6.6667000000000002E-3</v>
       </c>
-      <c r="C24" s="1">
+      <c r="D24" s="1">
         <v>2.7399999999999999E-5</v>
       </c>
-      <c r="D24" s="1">
+      <c r="E24" s="1">
         <v>0.11</v>
       </c>
-      <c r="E24" s="1">
+      <c r="F24" s="1">
         <v>-73.546666669999993</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="H24" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="1">
         <v>0.43</v>
       </c>
-      <c r="B25" s="1">
+      <c r="C25" s="1">
         <v>6.6667000000000002E-3</v>
       </c>
-      <c r="C25" s="1">
+      <c r="D25" s="1">
         <v>2.7399999999999999E-5</v>
       </c>
-      <c r="D25" s="1">
+      <c r="E25" s="1">
         <v>0.11</v>
       </c>
-      <c r="E25" s="1">
+      <c r="F25" s="1">
         <v>-89.716666669999995</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="H25" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="1">
         <v>6.3014000000000004E-3</v>
       </c>
-      <c r="B26" s="1">
+      <c r="C26" s="1">
         <v>6.6667000000000002E-3</v>
       </c>
-      <c r="C26" s="1">
+      <c r="D26" s="1">
         <v>2.7399999999999999E-5</v>
       </c>
-      <c r="D26" s="1">
+      <c r="E26" s="1">
         <v>0.11</v>
       </c>
-      <c r="E26" s="1">
+      <c r="F26" s="1">
         <v>-87.876666670000006</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="H26" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="1">
         <v>8.0999999999999996E-3</v>
       </c>
-      <c r="B27" s="1">
+      <c r="C27" s="1">
         <v>6.6667000000000002E-3</v>
       </c>
-      <c r="C27" s="1">
+      <c r="D27" s="1">
         <v>2.7399999999999999E-5</v>
       </c>
-      <c r="D27" s="1">
+      <c r="E27" s="1">
         <v>0.11</v>
       </c>
-      <c r="E27" s="1">
+      <c r="F27" s="1">
         <v>-88.246666669999996</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="H27" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="1">
         <v>100.5</v>
       </c>
-      <c r="B28" s="1">
+      <c r="C28" s="1">
         <v>0.3</v>
       </c>
-      <c r="C28" s="1">
+      <c r="D28" s="1">
         <v>0.33333000000000002</v>
       </c>
-      <c r="D28" s="1">
+      <c r="E28" s="1">
         <v>5.1999999999999995E-4</v>
       </c>
-      <c r="E28" s="1">
+      <c r="F28" s="1">
         <v>52.526666669999997</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="G28" s="1" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="1">
         <v>100.5</v>
       </c>
-      <c r="B29" s="1">
+      <c r="C29" s="1">
         <v>0.3</v>
       </c>
-      <c r="C29" s="1">
+      <c r="D29" s="1">
         <v>0.33333000000000002</v>
       </c>
-      <c r="D29" s="1">
+      <c r="E29" s="1">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="E29" s="1">
+      <c r="F29" s="1">
         <v>-85.36</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="G29" s="1" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="1">
         <v>165</v>
       </c>
-      <c r="B30" s="1">
+      <c r="C30" s="1">
         <v>0.3</v>
       </c>
-      <c r="C30" s="1">
+      <c r="D30" s="1">
         <v>0.33333000000000002</v>
       </c>
-      <c r="D30" s="1">
+      <c r="E30" s="1">
         <v>5.1999999999999995E-4</v>
       </c>
-      <c r="E30" s="1">
+      <c r="F30" s="1">
         <v>54.626666669999999</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="G30" s="1" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="1">
         <v>165</v>
       </c>
-      <c r="B31" s="1">
+      <c r="C31" s="1">
         <v>0.3</v>
       </c>
-      <c r="C31" s="1">
+      <c r="D31" s="1">
         <v>0.33333000000000002</v>
       </c>
-      <c r="D31" s="1">
+      <c r="E31" s="1">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="E31" s="1">
+      <c r="F31" s="1">
         <v>-85.45</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="G31" s="1" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="1">
         <v>0.33500000000000002</v>
       </c>
-      <c r="B32" s="1">
+      <c r="C32" s="1">
         <v>0.3</v>
       </c>
-      <c r="C32" s="1">
+      <c r="D32" s="1">
         <v>0.33333000000000002</v>
       </c>
-      <c r="D32" s="1">
+      <c r="E32" s="1">
         <v>5.1999999999999995E-4</v>
       </c>
-      <c r="E32" s="1">
+      <c r="F32" s="1">
         <v>84.596666670000005</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="G32" s="1" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="1">
         <v>0.33500000000000002</v>
       </c>
-      <c r="B33" s="1">
+      <c r="C33" s="1">
         <v>0.3</v>
       </c>
-      <c r="C33" s="1">
+      <c r="D33" s="1">
         <v>0.33333000000000002</v>
       </c>
-      <c r="D33" s="1">
+      <c r="E33" s="1">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="E33" s="1">
-        <v>84.596666670000005</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>16</v>
+      <c r="F33" s="1">
+        <v>79.214333300000007</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="1">
         <v>0.55000000000000004</v>
       </c>
-      <c r="B34" s="1">
+      <c r="C34" s="1">
         <v>0.3</v>
       </c>
-      <c r="C34" s="1">
+      <c r="D34" s="1">
         <v>0.33333000000000002</v>
       </c>
-      <c r="D34" s="1">
+      <c r="E34" s="1">
         <v>5.1999999999999995E-4</v>
       </c>
-      <c r="E34" s="1">
+      <c r="F34" s="1">
         <v>166.74333329999999</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="G34" s="1" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="1">
         <v>0.55000000000000004</v>
       </c>
-      <c r="B35" s="1">
+      <c r="C35" s="1">
         <v>0.3</v>
       </c>
-      <c r="C35" s="1">
+      <c r="D35" s="1">
         <v>0.33333000000000002</v>
       </c>
-      <c r="D35" s="1">
+      <c r="E35" s="1">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="E35" s="1">
+      <c r="F35" s="5">
         <v>-47.53</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
+      <c r="G35" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" s="1">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="B36" s="1">
+      <c r="C36" s="1">
         <v>0.14285999999999999</v>
       </c>
-      <c r="C36" s="1">
+      <c r="D36" s="1">
         <v>2.8570000000000002E-2</v>
       </c>
-      <c r="D36" s="1">
+      <c r="E36" s="1">
         <v>0.01</v>
       </c>
-      <c r="E36" s="1">
+      <c r="F36" s="1">
         <v>154.90666669999999</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G36" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="H36" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="1">
         <v>2.4</v>
       </c>
-      <c r="B37" s="1">
+      <c r="C37" s="1">
         <v>0.14285999999999999</v>
       </c>
-      <c r="C37" s="1">
+      <c r="D37" s="1">
         <v>2.8570000000000002E-2</v>
       </c>
-      <c r="D37" s="1">
+      <c r="E37" s="1">
         <v>0.01</v>
       </c>
-      <c r="E37" s="1">
+      <c r="F37" s="1">
         <v>-87.983333329999994</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G37" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="H37" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" s="1">
         <v>0.115</v>
       </c>
-      <c r="B38" s="1">
+      <c r="C38" s="1">
         <v>0.16667000000000001</v>
       </c>
-      <c r="C38" s="1">
+      <c r="D38" s="1">
         <v>0.2</v>
       </c>
-      <c r="D38" s="1">
+      <c r="E38" s="1">
         <v>0.03</v>
       </c>
-      <c r="E38" s="1">
+      <c r="F38" s="1">
         <v>213.47333330000001</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="G38" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G38" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="H38" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" s="1">
         <v>7.8</v>
       </c>
-      <c r="B39" s="1">
+      <c r="C39" s="1">
         <v>0.16667000000000001</v>
       </c>
-      <c r="C39" s="1">
+      <c r="D39" s="1">
         <v>0.2</v>
       </c>
-      <c r="D39" s="1">
+      <c r="E39" s="1">
         <v>0.03</v>
       </c>
-      <c r="E39" s="1">
+      <c r="F39" s="1">
         <v>-71.123333329999994</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G39" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="H39" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40" s="1">
         <v>21.84</v>
       </c>
-      <c r="B40" s="1">
+      <c r="C40" s="1">
         <v>0.16667000000000001</v>
       </c>
-      <c r="C40" s="1">
+      <c r="D40" s="1">
         <v>0.2</v>
       </c>
-      <c r="D40" s="1">
+      <c r="E40" s="1">
         <v>0.03</v>
       </c>
-      <c r="E40" s="1">
+      <c r="F40" s="1">
         <v>-75.946666669999999</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="G40" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G40" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="H40" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41" s="2">
         <v>6552</v>
       </c>
-      <c r="B41" s="1">
+      <c r="C41" s="1">
         <v>0.16667000000000001</v>
       </c>
-      <c r="C41" s="1">
+      <c r="D41" s="1">
         <v>0.2</v>
       </c>
-      <c r="D41" s="1">
+      <c r="E41" s="1">
         <v>0.03</v>
       </c>
-      <c r="E41" s="3">
+      <c r="F41" s="3">
         <v>-81.503332999999998</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="G41" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G41" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="1">
+      <c r="H41" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42" s="1">
         <v>1.6437999999999999E-3</v>
       </c>
-      <c r="B42" s="1">
+      <c r="C42" s="1">
         <v>7.1429999999999993E-2</v>
       </c>
-      <c r="C42" s="1">
+      <c r="D42" s="1">
         <v>1.3699000000000001E-3</v>
       </c>
-      <c r="D42" s="1">
+      <c r="E42" s="1">
         <v>0.03</v>
       </c>
-      <c r="E42" s="1">
+      <c r="F42" s="1">
         <v>72.323333329999997</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="G42" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G42" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="H42" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" s="1">
         <v>5.4795E-3</v>
       </c>
-      <c r="B43" s="1">
+      <c r="C43" s="1">
         <v>7.1429999999999993E-2</v>
       </c>
-      <c r="C43" s="1">
+      <c r="D43" s="1">
         <v>1.3699000000000001E-3</v>
       </c>
-      <c r="D43" s="1">
+      <c r="E43" s="1">
         <v>0.03</v>
       </c>
-      <c r="E43" s="1">
+      <c r="F43" s="1">
         <v>-96.562724009999997</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G43" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="H43" s="1" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1743,21 +1763,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5397B46-BE56-AF4D-83BF-852B6269BE57}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="10.83203125" style="4"/>
-    <col min="6" max="6" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="12.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="10.875" style="4"/>
+    <col min="6" max="6" width="9.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.375" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>58</v>
       </c>
@@ -1783,7 +1803,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>-4.4775557664936798</v>
       </c>
@@ -1809,7 +1829,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>-5.3187587626244124</v>
       </c>
@@ -1835,7 +1855,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>-2.8436628991291899</v>
       </c>
@@ -1861,7 +1881,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>-4.6777807052660805</v>
       </c>
@@ -1887,7 +1907,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>-4.5686362358410122</v>
       </c>
@@ -1913,7 +1933,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>-0.47495519296315469</v>
       </c>
@@ -1939,7 +1959,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>-0.47495519296315469</v>
       </c>
@@ -1965,7 +1985,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>-0.25963731050575611</v>
       </c>
@@ -1991,7 +2011,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>-0.25963731050575611</v>
       </c>
@@ -2017,7 +2037,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>-2.9520634838619206</v>
       </c>
@@ -2043,7 +2063,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>-2.9520634838619206</v>
       </c>
@@ -2069,7 +2089,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>-2.736766461560511</v>
       </c>
@@ -2095,7 +2115,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>-2.736766461560511</v>
       </c>
@@ -2121,7 +2141,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>-3.9718355805755299</v>
       </c>
@@ -2147,7 +2167,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>-2.0969100130080562</v>
       </c>
@@ -2173,7 +2193,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>-3.4164611807456473</v>
       </c>
@@ -2199,7 +2219,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>-1.585026652029182</v>
       </c>
@@ -2225,7 +2245,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>-1.1378686206869628</v>
       </c>
@@ -2251,7 +2271,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>1.3392526340326993</v>
       </c>
@@ -2277,7 +2297,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>-5.259637310505755</v>
       </c>
@@ -2303,7 +2323,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>-4.7375489102695703</v>
       </c>
@@ -2329,7 +2349,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>-1.9999999999999996</v>
       </c>
@@ -2355,7 +2375,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>-2.8436628991291899</v>
       </c>
@@ -2381,7 +2401,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>-0.36653154442041347</v>
       </c>
@@ -2407,7 +2427,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>-2.2005629513832825</v>
       </c>
@@ -2433,7 +2453,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>-2.09151498112135</v>
       </c>
@@ -2459,7 +2479,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>2.0021660617565074</v>
       </c>
@@ -2485,7 +2505,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>2.0021660617565074</v>
       </c>
@@ -2511,7 +2531,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>2.2174839442139058</v>
       </c>
@@ -2537,7 +2557,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>2.2174839442139058</v>
       </c>
@@ -2563,7 +2583,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>-0.47495519296315469</v>
       </c>
@@ -2589,7 +2609,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>-0.47495519296315469</v>
       </c>
@@ -2603,7 +2623,7 @@
         <v>-1.2365720064370627</v>
       </c>
       <c r="E33" s="1">
-        <v>84.596666670000005</v>
+        <v>79.214333300000007</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>16</v>
@@ -2615,7 +2635,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>-0.25963731050575611</v>
       </c>
@@ -2641,7 +2661,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>-0.25963731050575611</v>
       </c>
@@ -2667,7 +2687,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>-1.4948500216800937</v>
       </c>
@@ -2693,7 +2713,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>0.38021124171160597</v>
       </c>
@@ -2719,7 +2739,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>-0.9393021596463883</v>
       </c>
@@ -2745,7 +2765,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>0.89209460269048035</v>
       </c>
@@ -2771,7 +2791,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>1.3392526340326993</v>
       </c>
@@ -2797,7 +2817,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>3.8163738887523619</v>
       </c>
@@ -2823,7 +2843,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>-2.7841510238885454</v>
       </c>
@@ -2849,7 +2869,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>-2.2612590687324019</v>
       </c>

</xml_diff>